<commit_message>
Updating knapsack fractional problem after class E
</commit_message>
<xml_diff>
--- a/161702/presentation/10 - Greedy Algorithm 2/Knapsack Greedy.xlsx
+++ b/161702/presentation/10 - Greedy Algorithm 2/Knapsack Greedy.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7800" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7800" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="27">
   <si>
     <t>w</t>
   </si>
@@ -73,6 +75,39 @@
   </si>
   <si>
     <t>benefit</t>
+  </si>
+  <si>
+    <t>item</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>value (b/w)</t>
+  </si>
+  <si>
+    <t>w taken</t>
+  </si>
+  <si>
+    <t>w remaining</t>
+  </si>
+  <si>
+    <t>Max Weight = W = 10</t>
+  </si>
+  <si>
+    <t>Max Benefit</t>
+  </si>
+  <si>
+    <t>Ratio benefit/weight</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>weight remaining</t>
+  </si>
+  <si>
+    <t>Max weight = W = 10</t>
   </si>
 </sst>
 </file>
@@ -851,7 +886,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -957,7 +992,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" ref="F4:F7" si="1">F3-E4</f>
+        <f t="shared" ref="F4:F5" si="1">F3-E4</f>
         <v>0</v>
       </c>
       <c r="G4" s="1">
@@ -1010,4 +1045,780 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G33"/>
+  <sheetViews>
+    <sheetView topLeftCell="A20" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1">
+        <f>C2/B2</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1">
+        <v>32</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" ref="D3:D6" si="0">C3/B3</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1">
+        <v>40</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>6.666666666666667</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>30</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>50</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2">
+        <v>50</v>
+      </c>
+      <c r="D10" s="1">
+        <f>C10/B10</f>
+        <v>50</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <f>10-E10</f>
+        <v>9</v>
+      </c>
+      <c r="G10" s="1">
+        <f>E10/B10*C10</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>4</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2">
+        <v>30</v>
+      </c>
+      <c r="D11" s="1">
+        <f>C11/B11</f>
+        <v>15</v>
+      </c>
+      <c r="E11" s="1">
+        <v>2</v>
+      </c>
+      <c r="F11" s="1">
+        <f>F10-E11</f>
+        <v>7</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" ref="G11:G14" si="1">E11/B11*C11</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2">
+        <v>4</v>
+      </c>
+      <c r="C12" s="2">
+        <v>12</v>
+      </c>
+      <c r="D12" s="1">
+        <f>C12/B12</f>
+        <v>3</v>
+      </c>
+      <c r="E12" s="1">
+        <v>4</v>
+      </c>
+      <c r="F12" s="1">
+        <f t="shared" ref="F12:F14" si="2">F11-E12</f>
+        <v>3</v>
+      </c>
+      <c r="G12" s="1">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>3</v>
+      </c>
+      <c r="B13" s="1">
+        <v>6</v>
+      </c>
+      <c r="C13" s="1">
+        <v>40</v>
+      </c>
+      <c r="D13" s="1">
+        <f>C13/B13</f>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="E13" s="1">
+        <v>3</v>
+      </c>
+      <c r="F13" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1">
+        <v>8</v>
+      </c>
+      <c r="C14" s="1">
+        <v>32</v>
+      </c>
+      <c r="D14" s="1">
+        <f>C14/B14</f>
+        <v>4</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E15" s="1">
+        <f>SUM(E10:E14)</f>
+        <v>10</v>
+      </c>
+      <c r="G15" s="3">
+        <f>SUM(G10:G14)</f>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>5</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2">
+        <v>50</v>
+      </c>
+      <c r="D19" s="1">
+        <f>C19/B19</f>
+        <v>50</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1">
+        <f>10-E19</f>
+        <v>9</v>
+      </c>
+      <c r="G19" s="1">
+        <f>E19/B19*C19</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>3</v>
+      </c>
+      <c r="B20" s="2">
+        <v>6</v>
+      </c>
+      <c r="C20" s="2">
+        <v>40</v>
+      </c>
+      <c r="D20" s="1">
+        <f>C20/B20</f>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="E20" s="1">
+        <v>6</v>
+      </c>
+      <c r="F20" s="1">
+        <f>F19-E20</f>
+        <v>3</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" ref="G20:G23" si="3">E20/B20*C20</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>2</v>
+      </c>
+      <c r="B21" s="1">
+        <v>8</v>
+      </c>
+      <c r="C21" s="1">
+        <v>32</v>
+      </c>
+      <c r="D21" s="1">
+        <f>C21/B21</f>
+        <v>4</v>
+      </c>
+      <c r="E21" s="1">
+        <v>3</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" ref="F21:F23" si="4">F20-E21</f>
+        <v>0</v>
+      </c>
+      <c r="G21" s="1">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>4</v>
+      </c>
+      <c r="B22" s="1">
+        <v>2</v>
+      </c>
+      <c r="C22" s="1">
+        <v>30</v>
+      </c>
+      <c r="D22" s="1">
+        <f>C22/B22</f>
+        <v>15</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>1</v>
+      </c>
+      <c r="B23" s="1">
+        <v>4</v>
+      </c>
+      <c r="C23" s="1">
+        <v>12</v>
+      </c>
+      <c r="D23" s="1">
+        <f>C23/B23</f>
+        <v>3</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G23" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E24" s="1">
+        <f>SUM(E19:E23)</f>
+        <v>10</v>
+      </c>
+      <c r="G24" s="3">
+        <f>SUM(G19:G23)</f>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>5</v>
+      </c>
+      <c r="B28" s="2">
+        <v>1</v>
+      </c>
+      <c r="C28" s="2">
+        <v>50</v>
+      </c>
+      <c r="D28" s="1">
+        <f>C28/B28</f>
+        <v>50</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1</v>
+      </c>
+      <c r="F28" s="1">
+        <f>10-E28</f>
+        <v>9</v>
+      </c>
+      <c r="G28" s="1">
+        <f>E28/B28*C28</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>4</v>
+      </c>
+      <c r="B29" s="2">
+        <v>2</v>
+      </c>
+      <c r="C29" s="2">
+        <v>30</v>
+      </c>
+      <c r="D29" s="1">
+        <f>C29/B29</f>
+        <v>15</v>
+      </c>
+      <c r="E29" s="1">
+        <v>2</v>
+      </c>
+      <c r="F29" s="1">
+        <f>F28-E29</f>
+        <v>7</v>
+      </c>
+      <c r="G29" s="1">
+        <f t="shared" ref="G29:G32" si="5">E29/B29*C29</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>3</v>
+      </c>
+      <c r="B30" s="2">
+        <v>6</v>
+      </c>
+      <c r="C30" s="2">
+        <v>40</v>
+      </c>
+      <c r="D30" s="1">
+        <f>C30/B30</f>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="E30" s="1">
+        <v>6</v>
+      </c>
+      <c r="F30" s="1">
+        <f t="shared" ref="F30:F32" si="6">F29-E30</f>
+        <v>1</v>
+      </c>
+      <c r="G30" s="1">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>2</v>
+      </c>
+      <c r="B31" s="2">
+        <v>8</v>
+      </c>
+      <c r="C31" s="2">
+        <v>32</v>
+      </c>
+      <c r="D31" s="1">
+        <f>C31/B31</f>
+        <v>4</v>
+      </c>
+      <c r="E31" s="1">
+        <v>1</v>
+      </c>
+      <c r="F31" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G31" s="1">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>1</v>
+      </c>
+      <c r="B32" s="1">
+        <v>4</v>
+      </c>
+      <c r="C32" s="1">
+        <v>12</v>
+      </c>
+      <c r="D32" s="1">
+        <f>C32/B32</f>
+        <v>3</v>
+      </c>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G32" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E33" s="1">
+        <f>SUM(E28:E32)</f>
+        <v>10</v>
+      </c>
+      <c r="G33" s="3">
+        <f>SUM(G28:G32)</f>
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A28:D32">
+    <sortCondition descending="1" ref="D28:D32"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1">
+        <v>50</v>
+      </c>
+      <c r="D2" s="1">
+        <f>C2/B2</f>
+        <v>16.666666666666668</v>
+      </c>
+      <c r="E2" s="1">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1">
+        <f>10-E2</f>
+        <v>7</v>
+      </c>
+      <c r="G2" s="1">
+        <f>E2/B2*C2</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>40</v>
+      </c>
+      <c r="D3" s="1">
+        <f>C3/B3</f>
+        <v>10</v>
+      </c>
+      <c r="E3" s="1">
+        <v>4</v>
+      </c>
+      <c r="F3" s="1">
+        <f>F2-E3</f>
+        <v>3</v>
+      </c>
+      <c r="G3" s="1">
+        <f t="shared" ref="G3:G5" si="0">E3/B3*C3</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1">
+        <v>30</v>
+      </c>
+      <c r="D4" s="1">
+        <f>C4/B4</f>
+        <v>5</v>
+      </c>
+      <c r="E4" s="1">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" ref="F4:F7" si="1">F3-E4</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1">
+        <f>C5/B5</f>
+        <v>2</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E6" s="1">
+        <f>SUM(E2:E5)</f>
+        <v>10</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="3">
+        <f>SUM(G2:G5)</f>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="1"/>
+    </row>
+  </sheetData>
+  <sortState ref="A2:G5">
+    <sortCondition descending="1" ref="D2:D5"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>